<commit_message>
Added functionality to recognize different dashboard objects. Not completed
</commit_message>
<xml_diff>
--- a/automationTest/res/importFiles/ES-284/ES-284 - Step 4 - Aggregations - Test to Automate.xlsx
+++ b/automationTest/res/importFiles/ES-284/ES-284 - Step 4 - Aggregations - Test to Automate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mubari\eclipse\automationTest\res\importFiles\ES-284\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitRepository\automationTest\res\importFiles\ES-284\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1351,7 +1351,7 @@
   <dimension ref="A1:AV62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1603,7 +1603,7 @@
         <v>5000</v>
       </c>
       <c r="P13" s="6">
-        <v>10</v>
+        <v>4900</v>
       </c>
       <c r="Q13" s="6">
         <v>4800</v>
@@ -1696,7 +1696,7 @@
       </c>
       <c r="P14" s="6">
         <f t="shared" ref="P14:AH14" si="0">P13/10</f>
-        <v>1</v>
+        <v>490</v>
       </c>
       <c r="Q14" s="6">
         <f t="shared" si="0"/>
@@ -4243,7 +4243,7 @@
       </c>
       <c r="I43" s="108">
         <f>SUM(K43:AT43)</f>
-        <v>13701350</v>
+        <v>14214800</v>
       </c>
       <c r="J43" s="38"/>
       <c r="K43" s="103">
@@ -4268,7 +4268,7 @@
       </c>
       <c r="P43" s="38">
         <f t="shared" si="2"/>
-        <v>1050</v>
+        <v>514500</v>
       </c>
       <c r="Q43" s="38">
         <f t="shared" si="2"/>
@@ -4411,7 +4411,7 @@
       </c>
       <c r="I44" s="108">
         <f t="shared" ref="I44:I51" si="4">SUM(K44:AT44)</f>
-        <v>11161950</v>
+        <v>11553150</v>
       </c>
       <c r="J44" s="38"/>
       <c r="K44" s="103">
@@ -4436,7 +4436,7 @@
       </c>
       <c r="P44" s="38">
         <f t="shared" si="5"/>
-        <v>800</v>
+        <v>392000</v>
       </c>
       <c r="Q44" s="38">
         <f t="shared" si="5"/>
@@ -4580,7 +4580,7 @@
       </c>
       <c r="I45" s="108">
         <f t="shared" si="4"/>
-        <v>6968200</v>
+        <v>7237150</v>
       </c>
       <c r="J45" s="38"/>
       <c r="K45" s="103">
@@ -4605,7 +4605,7 @@
       </c>
       <c r="P45" s="38">
         <f t="shared" si="7"/>
-        <v>550</v>
+        <v>269500</v>
       </c>
       <c r="Q45" s="38">
         <f t="shared" si="7"/>
@@ -4749,7 +4749,7 @@
       </c>
       <c r="I46" s="108">
         <f t="shared" si="4"/>
-        <v>17.4908</v>
+        <v>18.1265</v>
       </c>
       <c r="J46" s="38"/>
       <c r="K46" s="103">
@@ -4774,7 +4774,7 @@
       </c>
       <c r="P46" s="38">
         <f t="shared" si="9"/>
-        <v>1.3000000000000002E-3</v>
+        <v>0.63700000000000001</v>
       </c>
       <c r="Q46" s="38">
         <f t="shared" si="9"/>
@@ -4918,7 +4918,7 @@
       </c>
       <c r="I47" s="108">
         <f t="shared" si="4"/>
-        <v>15.424200000000003</v>
+        <v>16.011000000000003</v>
       </c>
       <c r="J47" s="38"/>
       <c r="K47" s="103">
@@ -4943,7 +4943,7 @@
       </c>
       <c r="P47" s="38">
         <f t="shared" si="11"/>
-        <v>1.2000000000000001E-3</v>
+        <v>0.58800000000000008</v>
       </c>
       <c r="Q47" s="38">
         <f t="shared" si="11"/>
@@ -5087,7 +5087,7 @@
       </c>
       <c r="I48" s="108">
         <f t="shared" si="4"/>
-        <v>12.7277</v>
+        <v>13.265600000000001</v>
       </c>
       <c r="J48" s="38"/>
       <c r="K48" s="103">
@@ -5112,7 +5112,7 @@
       </c>
       <c r="P48" s="38">
         <f t="shared" si="13"/>
-        <v>1.1000000000000001E-3</v>
+        <v>0.53900000000000003</v>
       </c>
       <c r="Q48" s="38">
         <f t="shared" si="13"/>
@@ -5256,7 +5256,7 @@
       </c>
       <c r="I49" s="108">
         <f t="shared" si="4"/>
-        <v>13701367.490799999</v>
+        <v>14214818.126499997</v>
       </c>
       <c r="J49" s="42"/>
       <c r="K49" s="104">
@@ -5281,7 +5281,7 @@
       </c>
       <c r="P49" s="42">
         <f t="shared" si="15"/>
-        <v>1050.0012999999999</v>
+        <v>514500.63699999999</v>
       </c>
       <c r="Q49" s="42">
         <f t="shared" si="15"/>
@@ -5425,7 +5425,7 @@
       </c>
       <c r="I50" s="108">
         <f t="shared" si="4"/>
-        <v>11161965.4242</v>
+        <v>11553166.011</v>
       </c>
       <c r="J50" s="42"/>
       <c r="K50" s="104">
@@ -5450,7 +5450,7 @@
       </c>
       <c r="P50" s="42">
         <f t="shared" si="17"/>
-        <v>800.00120000000004</v>
+        <v>392000.58799999999</v>
       </c>
       <c r="Q50" s="42">
         <f t="shared" si="17"/>
@@ -5594,7 +5594,7 @@
       </c>
       <c r="I51" s="108">
         <f t="shared" si="4"/>
-        <v>6968212.7276999997</v>
+        <v>7237163.2656000005</v>
       </c>
       <c r="J51" s="42"/>
       <c r="K51" s="104">
@@ -5619,7 +5619,7 @@
       </c>
       <c r="P51" s="42">
         <f t="shared" si="19"/>
-        <v>550.00109999999995</v>
+        <v>269500.53899999999</v>
       </c>
       <c r="Q51" s="42">
         <f t="shared" si="19"/>
@@ -5779,7 +5779,7 @@
       </c>
       <c r="P52" s="16">
         <f t="shared" si="21"/>
-        <v>120.00139999999999</v>
+        <v>34350.686000000002</v>
       </c>
       <c r="Q52" s="16">
         <f t="shared" si="21"/>
@@ -5939,7 +5939,7 @@
       </c>
       <c r="P53" s="16">
         <f t="shared" si="22"/>
-        <v>20.000399999999999</v>
+        <v>9800.1959999999999</v>
       </c>
       <c r="Q53" s="16">
         <f t="shared" si="22"/>
@@ -6099,7 +6099,7 @@
       </c>
       <c r="P54" s="16">
         <f t="shared" si="23"/>
-        <v>50.000999999999998</v>
+        <v>24500.49</v>
       </c>
       <c r="Q54" s="16">
         <f t="shared" si="23"/>
@@ -6463,7 +6463,7 @@
       </c>
       <c r="I57" s="108">
         <f t="shared" ref="I57:I62" si="25">SUM(K57:AT57)</f>
-        <v>1032320</v>
+        <v>1042100</v>
       </c>
       <c r="J57" s="3"/>
       <c r="K57" s="103">
@@ -6488,7 +6488,7 @@
       </c>
       <c r="P57" s="38">
         <f t="shared" si="26"/>
-        <v>20</v>
+        <v>9800</v>
       </c>
       <c r="Q57" s="38">
         <f t="shared" si="26"/>
@@ -6634,7 +6634,7 @@
       </c>
       <c r="I58" s="108">
         <f t="shared" si="25"/>
-        <v>4929550</v>
+        <v>4954000</v>
       </c>
       <c r="J58" s="3"/>
       <c r="K58" s="103">
@@ -6659,7 +6659,7 @@
       </c>
       <c r="P58" s="38">
         <f t="shared" si="27"/>
-        <v>50</v>
+        <v>24500</v>
       </c>
       <c r="Q58" s="38">
         <f t="shared" si="27"/>
@@ -6807,7 +6807,7 @@
       </c>
       <c r="I59" s="108">
         <f t="shared" si="25"/>
-        <v>20.646400000000003</v>
+        <v>20.842000000000006</v>
       </c>
       <c r="J59" s="3"/>
       <c r="K59" s="103">
@@ -6832,7 +6832,7 @@
       </c>
       <c r="P59" s="38">
         <f t="shared" si="28"/>
-        <v>4.0000000000000002E-4</v>
+        <v>0.19600000000000001</v>
       </c>
       <c r="Q59" s="38">
         <f t="shared" si="28"/>
@@ -6980,7 +6980,7 @@
       </c>
       <c r="I60" s="108">
         <f t="shared" si="25"/>
-        <v>98.590999999999994</v>
+        <v>99.08</v>
       </c>
       <c r="J60" s="3"/>
       <c r="K60" s="103">
@@ -7005,7 +7005,7 @@
       </c>
       <c r="P60" s="38">
         <f t="shared" si="29"/>
-        <v>1E-3</v>
+        <v>0.49000000000000005</v>
       </c>
       <c r="Q60" s="38">
         <f t="shared" si="29"/>
@@ -7153,7 +7153,7 @@
       </c>
       <c r="I61" s="108">
         <f t="shared" si="25"/>
-        <v>1032340.6464</v>
+        <v>1042120.8419999999</v>
       </c>
       <c r="J61" s="3"/>
       <c r="K61" s="103">
@@ -7178,7 +7178,7 @@
       </c>
       <c r="P61" s="38">
         <f t="shared" si="30"/>
-        <v>20.000399999999999</v>
+        <v>9800.1959999999999</v>
       </c>
       <c r="Q61" s="38">
         <f t="shared" si="30"/>
@@ -7326,7 +7326,7 @@
       </c>
       <c r="I62" s="108">
         <f t="shared" si="25"/>
-        <v>4929648.591</v>
+        <v>4954099.08</v>
       </c>
       <c r="J62" s="3"/>
       <c r="K62" s="103">
@@ -7351,7 +7351,7 @@
       </c>
       <c r="P62" s="38">
         <f t="shared" si="32"/>
-        <v>50.000999999999998</v>
+        <v>24500.49</v>
       </c>
       <c r="Q62" s="38">
         <f t="shared" si="32"/>

</xml_diff>